<commit_message>
line break removed from figure 4.5
</commit_message>
<xml_diff>
--- a/ForDevelopers/Listoffigures.xlsx
+++ b/ForDevelopers/Listoffigures.xlsx
@@ -158,7 +158,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">My fault –Fixed in GitHub</t>
+      <t xml:space="preserve">This was my fault –Fixed in GitHub</t>
     </r>
   </si>
   <si>
@@ -168,7 +168,19 @@
     <t>4.5</t>
   </si>
   <si>
-    <t>Will, the right-hand distribution has the words in the same position as the left-hand distribution.  Do you think it might be clearer what we mean (that the entire shaded area is about 95%) if we had "of the distribution" on one line, so that the words spanned the shaded area?</t>
+    <r>
+      <t xml:space="preserve">Will, the right-hand distribution has the words in the same position as the left-hand distribution.  Do you think it might be clearer what we mean (that the entire shaded area is about 95%) if we had "of the distribution" on one line, so that the words spanned the shaded area? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF990099"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Done (I assume you mean just the right distribution.)</t>
+    </r>
   </si>
   <si>
     <t>4.6</t>
@@ -192,7 +204,19 @@
     <t>4.9</t>
   </si>
   <si>
-    <t>Will, same question as 4.3 -- the z was capitalized.  Do you want me to tell them to go back to the original figure or to change the z back to lowercase?</t>
+    <r>
+      <t xml:space="preserve">Will, same question as 4.3 -- the z was capitalized.  Do you want me to tell them to go back to the original figure or to change the z back to lowercase? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF990099"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Up to you; this one wasn't my fault.</t>
+    </r>
   </si>
   <si>
     <t>5.1</t>
@@ -904,7 +928,7 @@
   <dimension ref="A1:E169"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
     </sheetView>
@@ -1435,7 +1459,7 @@
       <c r="D36" s="5"/>
       <c r="E36" s="0"/>
     </row>
-    <row r="37" customFormat="false" ht="93.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>5</v>
       </c>
@@ -1489,7 +1513,7 @@
       </c>
       <c r="E40" s="0"/>
     </row>
-    <row r="41" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
comments on the rest of the proofs
</commit_message>
<xml_diff>
--- a/ForDevelopers/Listoffigures.xlsx
+++ b/ForDevelopers/Listoffigures.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="208">
   <si>
     <t>Figure or Table</t>
   </si>
@@ -315,6 +315,21 @@
     <t>7.4</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">I am asking them to go back to the figure as it was submitted.  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF990099"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">In my notes, we were going to ask them to add the *title*, “Population of 12 Scores”.  Instead it's a *caption*.</t>
+    </r>
+  </si>
+  <si>
     <t>Table </t>
   </si>
   <si>
@@ -327,31 +342,114 @@
     <t>8.1</t>
   </si>
   <si>
-    <t>APA style says the words in the axis label should be capitalized.  Will, do you want to instruct them to go back to the original figures?  Or do you want them to change those words back to being capitalized?</t>
+    <r>
+      <t xml:space="preserve">APA style says the words in the axis label should be capitalized.  Will, do you want to instruct them to go back to the original figures?  Or do you want them to change those words back to being capitalized?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF990099"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Go back, in addition to the capitalization, they need to fix things like the dark black font on the labels anyway. Also, the  minor grid lines are doubled again (like they were in the original Ch3 proofs).
+I'll call this “Disease Complex 8A”</t>
+    </r>
   </si>
   <si>
     <t>8.2</t>
   </si>
   <si>
-    <t>We need to tell them to use the original version of the figure.  Their changes, though minor, have shifted the z label lower on the figure, so now it is harder to tell that the z refers to the top number line and "Maze completion time" refers to the bottom number line.  Also, according to APA style, those words should be capitalized -- Maze Completion Time.  That's a detail I need to go back and check on all the figures and make sure that they haven't introduced an APA error.</t>
+    <r>
+      <t xml:space="preserve">We need to tell them to use the original version of the figure.  Their changes, though minor, have shifted the z label lower on the figure, so now it is harder to tell that the z refers to the top number line and "Maze completion time" refers to the bottom number line.  Also, according to APA style, those words should be capitalized -- Maze Completion Time.  That's a detail I need to go back and check on all the figures and make sure that they haven't introduced an APA error.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF990099"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Disease Complex 8A</t>
+    </r>
   </si>
   <si>
     <t>8.3</t>
   </si>
   <si>
-    <t>The publisher deleted the labels for the two shaded areas!!!  I have told them to go back to the figure as it was submitted.</t>
+    <r>
+      <t xml:space="preserve">The publisher deleted the labels for the two shaded areas!!!  I have told them to go back to the figure as it was submitted.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF990099"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Disease Complex 8A</t>
+    </r>
   </si>
   <si>
     <t>8.4</t>
   </si>
   <si>
-    <t>Even the label on the second number line has all three words capitalized</t>
+    <r>
+      <t xml:space="preserve">Even the label on the second number line has all three words capitalized
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF990099"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">A different guy most have worked on these.  The axis font is gray now, but the shaded colors have gone to hell.  These need to be the same shades of red &amp; blue, and the same transparencies.  It also adds these additional bright sub-borders.  I'll call this “
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF990099"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Disease Complex 8B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF990099"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">”</t>
+    </r>
   </si>
   <si>
     <t>8.5</t>
   </si>
   <si>
-    <t>Capitalization needed on the second number line</t>
+    <r>
+      <t xml:space="preserve">Capitalization needed on the second number line
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF990099"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Disease Complex 8A</t>
+    </r>
   </si>
   <si>
     <t>8.6</t>
@@ -360,7 +458,19 @@
     <t>8.7</t>
   </si>
   <si>
-    <t>They need to go back to the original figure.  The z label has been shifted lower on the figure, losing the connection with the first number line, and the second number line's label needs to be capitalized.</t>
+    <r>
+      <t xml:space="preserve">They need to go back to the original figure.  The z label has been shifted lower on the figure, losing the connection with the first number line, and the second number line's label needs to be capitalized.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF990099"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Disease Complex 8A</t>
+    </r>
   </si>
   <si>
     <t>8.8</t>
@@ -369,30 +479,94 @@
     <t>8.9</t>
   </si>
   <si>
-    <t>I emailed Ramya about how this figure was inconsistent with other figures in the chapter.  See how small the font is in some places.  Need to tell them to go back to the original figure.</t>
+    <r>
+      <t xml:space="preserve">I emailed Ramya about how this figure was inconsistent with other figures in the chapter.  See how small the font is in some places.  Need to tell them to go back to the original figure.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF990099"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Disease Complex 8B</t>
+    </r>
   </si>
   <si>
     <t>8.10</t>
   </si>
   <si>
-    <t>Maze Completion Time needs capitalization.  Will, please look at this one and see what you think.</t>
+    <r>
+      <t xml:space="preserve">Maze Completion Time needs capitalization.  Will, please look at this one and see what you think.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF990099"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Disease Complex 8A</t>
+    </r>
   </si>
   <si>
     <t>8.11</t>
   </si>
   <si>
-    <t>Maze Completion Time needs capitalization.  </t>
+    <r>
+      <t xml:space="preserve">Maze Completion Time needs capitalization.  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF990099"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Disease Complex 8A</t>
+    </r>
   </si>
   <si>
     <t>8.12</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">The tick marks inside the orange box got narrower.  Also, there's a floating tick mark on the right side “
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF990099"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Disease Complex 8C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF990099"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">”</t>
+    </r>
+  </si>
+  <si>
     <t>8.13</t>
   </si>
   <si>
     <t>8.14</t>
   </si>
   <si>
+    <t>Disease Complex 8C</t>
+  </si>
+  <si>
     <t>9.1</t>
   </si>
   <si>
@@ -402,31 +576,71 @@
     <t>9.2</t>
   </si>
   <si>
-    <t>The font is too small on the lower number line and not consistent with other figures.  Will, do you want them to make this change, or do you want me to tell them to go back to the original figure?</t>
+    <r>
+      <t xml:space="preserve">The font is too small on the lower number line and not consistent with other figures.  Will, do you want them to make this change, or do you want me to tell them to go back to the original figure?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF990099"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Disease Complex 8B
+I vote that they do them again, to help increase the change they chapter figures will be handled consistently.  For this reason, I say “do over” in response to most of the time you ask me.</t>
+    </r>
   </si>
   <si>
     <t>9.3</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Same question as 9.2
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF990099"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Disease Complex 8B</t>
+    </r>
+  </si>
+  <si>
+    <t>9.4</t>
+  </si>
+  <si>
+    <t>9.5</t>
+  </si>
+  <si>
+    <t>9.6</t>
+  </si>
+  <si>
     <t>Same question as 9.2</t>
   </si>
   <si>
-    <t>9.4</t>
-  </si>
-  <si>
-    <t>9.5</t>
-  </si>
-  <si>
-    <t>9.6</t>
-  </si>
-  <si>
     <t>Same feedback as Table 9.1</t>
   </si>
   <si>
     <t>9.7</t>
   </si>
   <si>
-    <t>The wrong figure appears here.  I sent the correct figure 9 Jan 2015.</t>
+    <r>
+      <t xml:space="preserve">The wrong figure appears here.  I sent the correct figure 9 Jan 2015.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF990099"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Disease Complex 8B</t>
+    </r>
   </si>
   <si>
     <t>9.8</t>
@@ -435,7 +649,19 @@
     <t>9.9</t>
   </si>
   <si>
-    <t>The z labels need to be italicized.  Will, should I have them do it or should I send the figure again?</t>
+    <r>
+      <t xml:space="preserve">The z labels need to be italicized.  Will, should I have them do it or should I send the figure again?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF990099"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">The “2.33” got moved down.</t>
+    </r>
   </si>
   <si>
     <t>9.10</t>
@@ -447,6 +673,9 @@
     <t>10.1</t>
   </si>
   <si>
+    <t>Has those old ch3 problems with gridlines.</t>
+  </si>
+  <si>
     <t>10.2</t>
   </si>
   <si>
@@ -456,6 +685,21 @@
     <t>10.3</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Same, plus now the lines aren't clipped, so you see lines below x=0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
     <t>10.4</t>
   </si>
   <si>
@@ -480,7 +724,19 @@
     <t>11.4</t>
   </si>
   <si>
-    <t>Need to capitalize the labels</t>
+    <r>
+      <t xml:space="preserve">Need to capitalize the labels
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF990099"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Has those old ch3 problems with gridlines.</t>
+    </r>
   </si>
   <si>
     <t>12.1</t>
@@ -489,7 +745,19 @@
     <t>Have told them to move the word Condition so that it appears above the group names</t>
   </si>
   <si>
-    <t>Will:  Make sure you are OK with how the gridlines appear</t>
+    <r>
+      <t xml:space="preserve">Will:  Make sure you are OK with how the gridlines appear
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF990099"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Has those old ch3 problems with gridlines</t>
+    </r>
   </si>
   <si>
     <t>12.3</t>
@@ -504,7 +772,19 @@
     <t>12.6</t>
   </si>
   <si>
-    <t>This figure was badly cropped.  I told them to go back to the original figure.</t>
+    <r>
+      <t xml:space="preserve">This figure was badly cropped.  I told them to go back to the original figure.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF990099"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Has those old ch3 problems with gridlines</t>
+    </r>
   </si>
   <si>
     <t>12.7</t>
@@ -516,9 +796,15 @@
     <t>12.8</t>
   </si>
   <si>
+    <t>Has those old ch3 problems with gridlines</t>
+  </si>
+  <si>
     <t>12.9</t>
   </si>
   <si>
+    <t>Has those old ch3 problems with gridlines, and point borders.</t>
+  </si>
+  <si>
     <t>Same question about fonts</t>
   </si>
   <si>
@@ -537,6 +823,9 @@
     <t>13.1</t>
   </si>
   <si>
+    <t>Has those old ch3 problems with gridlines -like all the figures in this chapter</t>
+  </si>
+  <si>
     <t>13.2</t>
   </si>
   <si>
@@ -591,7 +880,20 @@
     <t>14.2</t>
   </si>
   <si>
-    <t>Font looks too small.  Will, should I re-send the figure?</t>
+    <r>
+      <t xml:space="preserve">Font looks too small.  Will, should I re-send the figure?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF990099"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">I vote 'yes', since they have to redo it anyway.</t>
+    </r>
   </si>
   <si>
     <t>14.3</t>
@@ -928,15 +1230,15 @@
   <dimension ref="A1:E169"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
+      <selection pane="bottomLeft" activeCell="D140" activeCellId="0" sqref="D139:D140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.61133603238866"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="4.62753036437247"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="13.5627530364372"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="5.40080971659919"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="53.668016194332"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="55.5506072874494"/>
@@ -1857,7 +2159,7 @@
       </c>
       <c r="E66" s="0"/>
     </row>
-    <row r="67" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
         <v>5</v>
       </c>
@@ -1866,13 +2168,13 @@
       </c>
       <c r="C67" s="0"/>
       <c r="D67" s="5" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="E67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B68" s="9" t="s">
         <v>73</v>
@@ -1885,7 +2187,7 @@
     </row>
     <row r="69" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B69" s="9" t="s">
         <v>75</v>
@@ -1901,7 +2203,7 @@
         <v>5</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C70" s="0"/>
       <c r="D70" s="5" t="s">
@@ -1914,7 +2216,7 @@
         <v>5</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C71" s="0"/>
       <c r="D71" s="5" t="s">
@@ -1922,267 +2224,273 @@
       </c>
       <c r="E71" s="0"/>
     </row>
-    <row r="72" customFormat="false" ht="62.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="157.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C72" s="0"/>
       <c r="D72" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E72" s="0"/>
     </row>
-    <row r="73" customFormat="false" ht="140.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="143.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C73" s="0"/>
       <c r="D73" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E73" s="0"/>
     </row>
-    <row r="74" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C74" s="0"/>
       <c r="D74" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E74" s="0"/>
     </row>
-    <row r="75" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="129.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E75" s="0"/>
     </row>
-    <row r="76" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C76" s="0"/>
       <c r="D76" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E76" s="0"/>
     </row>
-    <row r="77" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C77" s="0"/>
       <c r="D77" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E77" s="0"/>
     </row>
-    <row r="78" customFormat="false" ht="62.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E78" s="0"/>
     </row>
-    <row r="79" customFormat="false" ht="62.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C79" s="0"/>
       <c r="D79" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E79" s="0"/>
     </row>
-    <row r="80" customFormat="false" ht="62.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C80" s="0"/>
       <c r="D80" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E80" s="0"/>
     </row>
-    <row r="81" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C81" s="0"/>
       <c r="D81" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E81" s="0"/>
     </row>
-    <row r="82" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C82" s="0"/>
       <c r="D82" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E82" s="0"/>
     </row>
-    <row r="83" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D83" s="5"/>
+      <c r="D83" s="6" t="s">
+        <v>104</v>
+      </c>
       <c r="E83" s="0"/>
     </row>
-    <row r="84" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C84" s="0"/>
       <c r="D84" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E84" s="0"/>
     </row>
-    <row r="85" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D85" s="5"/>
+      <c r="D85" s="7" t="s">
+        <v>107</v>
+      </c>
       <c r="E85" s="0"/>
     </row>
-    <row r="86" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="8" t="s">
         <v>51</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C86" s="0"/>
       <c r="D86" s="5" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E86" s="0"/>
     </row>
-    <row r="87" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D87" s="5"/>
+      <c r="D87" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="E87" s="0"/>
     </row>
-    <row r="88" customFormat="false" ht="62.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="129.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C88" s="0"/>
       <c r="D88" s="5" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E88" s="0"/>
     </row>
-    <row r="89" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C89" s="0"/>
       <c r="D89" s="5" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E89" s="0"/>
     </row>
-    <row r="90" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C90" s="0"/>
       <c r="D90" s="5" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E90" s="0"/>
     </row>
-    <row r="91" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C91" s="0"/>
       <c r="D91" s="5" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E91" s="0"/>
     </row>
@@ -2191,11 +2499,11 @@
         <v>5</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C92" s="0"/>
       <c r="D92" s="5" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E92" s="0"/>
     </row>
@@ -2204,50 +2512,50 @@
         <v>51</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C93" s="0"/>
       <c r="D93" s="5" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="E93" s="0"/>
     </row>
-    <row r="94" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C94" s="0"/>
       <c r="D94" s="5" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="E94" s="0"/>
     </row>
-    <row r="95" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C95" s="0"/>
       <c r="D95" s="5" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="E95" s="0"/>
     </row>
-    <row r="96" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C96" s="0"/>
       <c r="D96" s="5" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="E96" s="0"/>
     </row>
@@ -2256,38 +2564,42 @@
         <v>5</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C97" s="0"/>
       <c r="D97" s="5" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E97" s="0"/>
     </row>
-    <row r="98" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D98" s="5"/>
+      <c r="D98" s="7" t="s">
+        <v>107</v>
+      </c>
       <c r="E98" s="0"/>
     </row>
-    <row r="99" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D99" s="5"/>
+      <c r="D99" s="6" t="s">
+        <v>127</v>
+      </c>
       <c r="E99" s="0"/>
     </row>
     <row r="100" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2295,119 +2607,129 @@
         <v>5</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C100" s="0"/>
       <c r="D100" s="5" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="E100" s="0"/>
     </row>
-    <row r="101" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D101" s="5"/>
+      <c r="D101" s="6" t="s">
+        <v>131</v>
+      </c>
       <c r="E101" s="0"/>
     </row>
-    <row r="102" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D102" s="5"/>
+      <c r="D102" s="6" t="s">
+        <v>127</v>
+      </c>
       <c r="E102" s="0"/>
     </row>
     <row r="103" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D103" s="5"/>
       <c r="E103" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B104" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D104" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C104" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D104" s="5"/>
       <c r="E104" s="0"/>
     </row>
-    <row r="105" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D105" s="5"/>
+      <c r="D105" s="6" t="s">
+        <v>127</v>
+      </c>
       <c r="E105" s="0"/>
     </row>
-    <row r="106" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D106" s="5"/>
+      <c r="D106" s="6" t="s">
+        <v>127</v>
+      </c>
       <c r="E106" s="0"/>
     </row>
     <row r="107" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D107" s="5"/>
       <c r="E107" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="8" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C108" s="0"/>
       <c r="D108" s="5" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="E108" s="0"/>
     </row>
@@ -2416,15 +2738,15 @@
         <v>5</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C109" s="9"/>
       <c r="D109" s="5" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E109" s="0"/>
     </row>
-    <row r="110" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
         <v>5</v>
       </c>
@@ -2435,65 +2757,65 @@
         <v>6</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="E110" s="0"/>
     </row>
-    <row r="111" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="E111" s="0"/>
     </row>
-    <row r="112" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="E112" s="0"/>
     </row>
-    <row r="113" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="E113" s="0"/>
     </row>
-    <row r="114" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="C114" s="0"/>
       <c r="D114" s="5" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="E114" s="0"/>
     </row>
@@ -2502,59 +2824,63 @@
         <v>5</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="C115" s="0"/>
       <c r="D115" s="5" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="E115" s="0"/>
     </row>
-    <row r="116" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D116" s="5"/>
+      <c r="D116" s="7" t="s">
+        <v>152</v>
+      </c>
       <c r="E116" s="0"/>
     </row>
-    <row r="117" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D117" s="5"/>
+      <c r="D117" s="7" t="s">
+        <v>154</v>
+      </c>
       <c r="E117" s="0"/>
     </row>
-    <row r="118" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="8" t="s">
         <v>51</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C118" s="0"/>
       <c r="D118" s="5"/>
       <c r="E118" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>6</v>
@@ -2562,12 +2888,12 @@
       <c r="D119" s="5"/>
       <c r="E119" s="0"/>
     </row>
-    <row r="120" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>6</v>
@@ -2580,7 +2906,7 @@
         <v>5</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>6</v>
@@ -2588,30 +2914,34 @@
       <c r="D121" s="5"/>
       <c r="E121" s="0"/>
     </row>
-    <row r="122" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D122" s="5"/>
+      <c r="D122" s="7" t="s">
+        <v>154</v>
+      </c>
       <c r="E122" s="0"/>
     </row>
-    <row r="123" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D123" s="5"/>
+      <c r="D123" s="7" t="s">
+        <v>161</v>
+      </c>
       <c r="E123" s="1" t="s">
         <v>49</v>
       </c>
@@ -2621,7 +2951,7 @@
         <v>5</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>6</v>
@@ -2634,7 +2964,7 @@
         <v>5</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>6</v>
@@ -2647,13 +2977,13 @@
         <v>5</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="E126" s="0"/>
     </row>
@@ -2662,7 +2992,7 @@
         <v>5</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>6</v>
@@ -2675,7 +3005,7 @@
         <v>5</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>6</v>
@@ -2688,7 +3018,7 @@
         <v>5</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>6</v>
@@ -2701,7 +3031,7 @@
         <v>5</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>6</v>
@@ -2714,7 +3044,7 @@
         <v>5</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>6</v>
@@ -2727,7 +3057,7 @@
         <v>5</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>6</v>
@@ -2740,14 +3070,14 @@
         <v>5</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D133" s="0"/>
       <c r="E133" s="1" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2755,14 +3085,14 @@
         <v>5</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D134" s="0"/>
       <c r="E134" s="1" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2770,14 +3100,14 @@
         <v>5</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D135" s="0"/>
       <c r="E135" s="1" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2785,14 +3115,14 @@
         <v>5</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D136" s="0"/>
       <c r="E136" s="1" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2800,12 +3130,12 @@
         <v>51</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="C137" s="0"/>
       <c r="D137" s="0"/>
       <c r="E137" s="1" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2813,37 +3143,39 @@
         <v>51</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="C138" s="0"/>
       <c r="D138" s="0"/>
       <c r="E138" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="139" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="C139" s="0"/>
-      <c r="D139" s="0"/>
+      <c r="D139" s="7" t="s">
+        <v>161</v>
+      </c>
       <c r="E139" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="C140" s="0"/>
-      <c r="D140" s="1" t="s">
-        <v>171</v>
+      <c r="D140" s="5" t="s">
+        <v>180</v>
       </c>
       <c r="E140" s="0"/>
     </row>
@@ -2852,25 +3184,25 @@
         <v>51</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="C141" s="0"/>
       <c r="D141" s="0"/>
       <c r="E141" s="1" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B142" s="9" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="C142" s="0"/>
       <c r="D142" s="0"/>
       <c r="E142" s="1" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2878,12 +3210,12 @@
         <v>51</v>
       </c>
       <c r="B143" s="9" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="C143" s="0"/>
       <c r="D143" s="0"/>
       <c r="E143" s="1" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2891,12 +3223,12 @@
         <v>51</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="C144" s="0"/>
       <c r="D144" s="0"/>
       <c r="E144" s="1" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2904,12 +3236,12 @@
         <v>51</v>
       </c>
       <c r="B145" s="9" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="C145" s="0"/>
       <c r="D145" s="0"/>
       <c r="E145" s="1" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2917,12 +3249,12 @@
         <v>51</v>
       </c>
       <c r="B146" s="9" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="C146" s="0"/>
       <c r="D146" s="0"/>
       <c r="E146" s="1" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2930,7 +3262,7 @@
         <v>5</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>6</v>
@@ -2943,7 +3275,7 @@
         <v>5</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>6</v>
@@ -2956,7 +3288,7 @@
         <v>5</v>
       </c>
       <c r="B149" s="9" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>6</v>
@@ -2969,12 +3301,12 @@
         <v>51</v>
       </c>
       <c r="B150" s="9" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="C150" s="0"/>
       <c r="D150" s="0"/>
       <c r="E150" s="1" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2982,12 +3314,12 @@
         <v>51</v>
       </c>
       <c r="B151" s="9" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="C151" s="0"/>
       <c r="D151" s="0"/>
       <c r="E151" s="1" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2995,7 +3327,7 @@
         <v>5</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="C152" s="0"/>
       <c r="D152" s="0"/>
@@ -3006,12 +3338,12 @@
         <v>51</v>
       </c>
       <c r="B153" s="9" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="C153" s="0"/>
       <c r="D153" s="0"/>
       <c r="E153" s="1" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3019,29 +3351,29 @@
         <v>5</v>
       </c>
       <c r="B154" s="9" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D154" s="0"/>
       <c r="E154" s="1" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="8" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B155" s="9" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D155" s="0"/>
       <c r="E155" s="5" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3049,14 +3381,14 @@
         <v>5</v>
       </c>
       <c r="B156" s="9" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D156" s="0"/>
       <c r="E156" s="5" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3064,7 +3396,7 @@
         <v>5</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>6</v>
@@ -3074,15 +3406,15 @@
     </row>
     <row r="158" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="8" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B158" s="9" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="C158" s="0"/>
       <c r="D158" s="0"/>
       <c r="E158" s="1" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3090,12 +3422,12 @@
         <v>5</v>
       </c>
       <c r="B159" s="9" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="C159" s="0"/>
       <c r="D159" s="0"/>
       <c r="E159" s="1" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3103,12 +3435,12 @@
         <v>5</v>
       </c>
       <c r="B160" s="9" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="C160" s="0"/>
       <c r="D160" s="0"/>
       <c r="E160" s="1" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3116,12 +3448,12 @@
         <v>51</v>
       </c>
       <c r="B161" s="9" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="C161" s="0"/>
       <c r="D161" s="0"/>
       <c r="E161" s="1" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3129,7 +3461,7 @@
         <v>51</v>
       </c>
       <c r="B162" s="9" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="C162" s="0"/>
       <c r="D162" s="0"/>
@@ -3140,12 +3472,12 @@
         <v>51</v>
       </c>
       <c r="B163" s="9" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="C163" s="0"/>
       <c r="D163" s="0"/>
       <c r="E163" s="1" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3153,14 +3485,14 @@
         <v>5</v>
       </c>
       <c r="B164" s="9" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="C164" s="0"/>
       <c r="D164" s="5" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3168,12 +3500,12 @@
         <v>5</v>
       </c>
       <c r="B165" s="9" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="C165" s="0"/>
       <c r="D165" s="0"/>
       <c r="E165" s="1" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3181,12 +3513,12 @@
         <v>5</v>
       </c>
       <c r="B166" s="9" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="C166" s="0"/>
       <c r="D166" s="0"/>
       <c r="E166" s="5" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3194,12 +3526,12 @@
         <v>5</v>
       </c>
       <c r="B167" s="9" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="C167" s="0"/>
       <c r="D167" s="0"/>
       <c r="E167" s="1" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3207,23 +3539,23 @@
         <v>5</v>
       </c>
       <c r="B168" s="9" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="C168" s="0"/>
       <c r="D168" s="0"/>
       <c r="E168" s="1" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="C169" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>